<commit_message>
added work item update
</commit_message>
<xml_diff>
--- a/AcmeWorkItems4/Data/Temp/workitemstemp.xlsx
+++ b/AcmeWorkItems4/Data/Temp/workitemstemp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test\Desktop\w\code projects\github projects\UiPath\AcmeWorkItems4\Data\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF62D533-E9FE-4DF8-99CD-8CD88CE138C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB5E3DD-03AF-4F72-AA7F-C8AA7D7CA45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24855" yWindow="1620" windowWidth="21600" windowHeight="11235" xr2:uid="{9DFB0EF2-EC0B-40E0-A7ED-A7B5223F926F}"/>
+    <workbookView xWindow="-24855" yWindow="1620" windowWidth="21600" windowHeight="11235" xr2:uid="{367D69D8-7CBB-48F2-869C-3A82D7564AB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -847,7 +847,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE1464B-98A9-4AD2-B4F0-AA60230BA55C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89C3DD0-2DCD-421E-AE18-26F68BAAF7C2}">
   <dimension ref="A1:G136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>